<commit_message>
PDQm 3.2.0 release for TI
</commit_message>
<xml_diff>
--- a/ITI/PDQm/StructureDefinition-IHE.PDQm.Match.Audit.Consumer.xlsx
+++ b/ITI/PDQm/StructureDefinition-IHE.PDQm.Match.Audit.Consumer.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.1.0</t>
+    <t>3.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-02T14:47:10-06:00</t>
+    <t>2025-11-04T12:09:52-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -390,7 +390,7 @@
     <t>A human language.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
+    <t>http://hl7.org/fhir/ValueSet/languages|4.0.1</t>
   </si>
   <si>
     <t>Resource.language</t>
@@ -515,7 +515,7 @@
     <t>Type of event.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/audit-event-type</t>
+    <t>http://hl7.org/fhir/ValueSet/audit-event-type|4.0.1</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -551,7 +551,7 @@
     <t>Sub-type of event.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/audit-event-sub-type</t>
+    <t>http://hl7.org/fhir/ValueSet/audit-event-sub-type|4.0.1</t>
   </si>
   <si>
     <t xml:space="preserve">value:$this}
@@ -783,7 +783,7 @@
     <t>An agent can be a person, an organization, software, device, or other actors that may be ascribed responsibility.</t>
   </si>
   <si>
-    <t xml:space="preserve">pattern:type}
+    <t xml:space="preserve">value:type}
 </t>
   </si>
   <si>
@@ -861,7 +861,7 @@
     <t>The Participation type of the agent to the event.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/participation-role-type</t>
+    <t>http://hl7.org/fhir/ValueSet/participation-role-type|4.0.1</t>
   </si>
   <si>
     <t>Event.performer.function</t>
@@ -900,7 +900,7 @@
     <t>What security role enabled the agent to participate in the event.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/security-role-type</t>
+    <t>http://hl7.org/fhir/ValueSet/security-role-type|4.0.1</t>
   </si>
   <si>
     <t>.role</t>
@@ -916,7 +916,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(PractitionerRole|Practitioner|Organization|Device|Patient|RelatedPerson)
+    <t xml:space="preserve">Reference(PractitionerRole|4.0.1|Practitioner|4.0.1|Organization|4.0.1|Device|4.0.1|Patient|4.0.1|RelatedPerson|4.0.1)
 </t>
   </si>
   <si>
@@ -1011,7 +1011,7 @@
     <t>AuditEvent.agent.location</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Location)
+    <t xml:space="preserve">Reference(Location|4.0.1)
 </t>
   </si>
   <si>
@@ -1078,7 +1078,7 @@
     <t>Used when the event is about exporting/importing onto media.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/dicm-405-mediatype</t>
+    <t>http://hl7.org/fhir/ValueSet/dicm-405-mediatype|4.0.1</t>
   </si>
   <si>
     <t>.player.description.mediaType</t>
@@ -1484,7 +1484,7 @@
     <t>Code specifying the type of system that detected and recorded the event.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/audit-source-type</t>
+    <t>http://hl7.org/fhir/ValueSet/audit-source-type|4.0.1</t>
   </si>
   <si>
     <t>.code</t>
@@ -1540,7 +1540,7 @@
     <t>AuditEvent.entity.what</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Resource)
+    <t xml:space="preserve">Reference(Resource|4.0.1)
 </t>
   </si>
   <si>
@@ -1574,7 +1574,7 @@
     <t>Code for the entity type involved in the audit event.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/audit-entity-type</t>
+    <t>http://hl7.org/fhir/ValueSet/audit-entity-type|4.0.1</t>
   </si>
   <si>
     <t>[self::Act].code or role.player.code</t>
@@ -1604,7 +1604,7 @@
     <t>Code representing the role the entity played in the audit event.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/object-role</t>
+    <t>http://hl7.org/fhir/ValueSet/object-role|4.0.1</t>
   </si>
   <si>
     <t>role.code (not sure what this would mean for an Act)</t>
@@ -1634,7 +1634,7 @@
     <t>Institutional policies for privacy and security may optionally fall under different accountability rules based on data life cycle. This provides a differentiating value for those cases.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/object-lifecycle-events</t>
+    <t>http://hl7.org/fhir/ValueSet/object-lifecycle-events|4.0.1</t>
   </si>
   <si>
     <t>target of ObservationEvent[code="lifecycle"].value</t>
@@ -1664,7 +1664,7 @@
     <t>Security Labels from the Healthcare Privacy and Security Classification System.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/security-labels</t>
+    <t>http://hl7.org/fhir/ValueSet/security-labels|4.0.1</t>
   </si>
   <si>
     <t>.confidentialityCode</t>
@@ -1883,7 +1883,7 @@
     <t>Aa resource (or, for logical models, the URI of the logical model).</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/resource-types</t>
+    <t>http://hl7.org/fhir/ValueSet/resource-types|4.0.1</t>
   </si>
   <si>
     <t>Reference.type</t>
@@ -1980,7 +1980,7 @@
     <t>A coded type for an identifier that can be used to determine which identifier to use for a specific purpose.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/identifier-type</t>
+    <t>http://hl7.org/fhir/ValueSet/identifier-type|4.0.1</t>
   </si>
   <si>
     <t>Identifier.type</t>
@@ -2061,7 +2061,7 @@
     <t>AuditEvent.entity.what.identifier.assigner</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization)
+    <t xml:space="preserve">Reference(Organization|4.0.1)
 </t>
   </si>
   <si>
@@ -2638,17 +2638,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="50.49609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="41.4609375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.15234375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="45.28515625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="37.18359375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.00390625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="34.8125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.29296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.21484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.55078125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.1171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.75390625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="78.44140625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="99.77734375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2657,28 +2657,28 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="38.8125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="95.56640625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="51.44921875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="34.80859375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.08984375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="14.4296875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="15.31640625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="85.70703125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="47.26171875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.10546875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.6953125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="35.90625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.44140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="30.5546875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="8.51953125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="8.859375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="26.71875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="155.37890625" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="49.390625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="34.4140625" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="40.00390625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="23.9609375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="139.34765625" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="44.29296875" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="29.45703125" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="30.86328125" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="35.875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -12907,7 +12907,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="86" hidden="true">
+    <row r="86">
       <c r="A86" t="s" s="2">
         <v>422</v>
       </c>
@@ -13271,7 +13271,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="89" hidden="true">
+    <row r="89">
       <c r="A89" t="s" s="2">
         <v>425</v>
       </c>
@@ -14593,7 +14593,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="100" hidden="true">
+    <row r="100">
       <c r="A100" t="s" s="2">
         <v>437</v>
       </c>
@@ -14713,7 +14713,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="101" hidden="true">
+    <row r="101">
       <c r="A101" t="s" s="2">
         <v>438</v>
       </c>
@@ -25921,12 +25921,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AP193">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>